<commit_message>
Added a venv activation into ф Django commands file
</commit_message>
<xml_diff>
--- a/Elegant Python.xlsx
+++ b/Elegant Python.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Strings" sheetId="1" r:id="rId1"/>
     <sheet name="List, Dict" sheetId="2" r:id="rId2"/>
+    <sheet name="pipes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>+</t>
   </si>
@@ -41,9 +42,6 @@
   </si>
   <si>
     <t>Назначение</t>
-  </si>
-  <si>
-    <t>Пример</t>
   </si>
   <si>
     <t>[::-1]</t>
@@ -101,18 +99,168 @@
   </si>
   <si>
     <t>d = [[x] for x in List_of_variants]</t>
+  </si>
+  <si>
+    <t>Объединение 2 словарей. Если ключи совпадают, значение в него вписывается из последнего словаря</t>
+  </si>
+  <si>
+    <t>d = {**dict1, **dict2}</t>
+  </si>
+  <si>
+    <t>Объединение 2 словарей, начиная с Питона 3.9</t>
+  </si>
+  <si>
+    <t>d = dict1 | dict2,       dict3 |=dict2</t>
+  </si>
+  <si>
+    <t>"dfgdfggdf"'.removeprefix(' " ').removesuffix(' " ')</t>
+  </si>
+  <si>
+    <t>Удаление первого и конечного вхождения элемента</t>
+  </si>
+  <si>
+    <t>Код, пример</t>
+  </si>
+  <si>
+    <t>from pipe import *</t>
+  </si>
+  <si>
+    <t>[1,2,3,4] | where(lambda x: x&lt;=2) | as_list</t>
+  </si>
+  <si>
+    <t>Format строки в питоне 3.7, нужные значения вставляем прямо в фигурные скобки</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">f"Ответ будет равен:   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {d + 20}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Ответ будет равен: {}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.format(d+20)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Ответы равны: a = {}, b = {}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.format(a,b)
+"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ответы равны: второй ответ b = {2}, первый ответ a = {1}, третий ответ c = {3}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.format(a,b,c)</t>
+    </r>
+  </si>
+  <si>
+    <t>Format строки в питоне до 3.7, нужные значения вставляем в аргументы фунции format. Если надо, можно сделать нумерованные места в строке.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -144,6 +292,14 @@
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -185,30 +341,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -491,76 +656,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="41" style="8" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="45.42578125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="41" style="8" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,10 +826,10 @@
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -596,51 +842,59 @@
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
@@ -753,13 +1007,95 @@
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Many additions about Docker and Linux
</commit_message>
<xml_diff>
--- a/Elegant Python.xlsx
+++ b/Elegant Python.xlsx
@@ -33,9 +33,6 @@
     <t>a + b  -&gt;   HelloPython</t>
   </si>
   <si>
-    <t>Создать словарь из существующиего по условию к значениям или ключам</t>
-  </si>
-  <si>
     <t>{k: v for k, v in &lt;начальный dict&gt;.iteritems() if v[0] &lt; 5 and v[1] &lt; 5}</t>
   </si>
   <si>
@@ -529,18 +526,29 @@
       </rPr>
       <t xml:space="preserve">   ПОРЯДОК for - обратный!</t>
     </r>
+  </si>
+  <si>
+    <t>Создать словарь из существующего по условию к значениям или ключам</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -690,40 +698,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1029,13 +1037,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,32 +1059,32 @@
     </row>
     <row r="3" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1086,18 +1094,18 @@
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1162,7 +1170,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,90 +1182,90 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1393,21 +1401,21 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5"/>
     </row>
@@ -1480,18 +1488,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
A huge addition to Pandas
</commit_message>
<xml_diff>
--- a/Elegant Python.xlsx
+++ b/Elegant Python.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Strings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
   <si>
     <t>+</t>
   </si>
@@ -87,9 +87,6 @@
     <t>применяет функцию func к каждому элементу given_list и выдает лист результатов</t>
   </si>
   <si>
-    <t>d = [[] for x in xrange(n)]</t>
-  </si>
-  <si>
     <t>Создать пустой Лист Листов</t>
   </si>
   <si>
@@ -529,6 +526,62 @@
   </si>
   <si>
     <t>Создать словарь из существующего по условию к значениям или ключам</t>
+  </si>
+  <si>
+    <t>d = [[] for x in range(n)]</t>
+  </si>
+  <si>
+    <t>x = lambda a, b: a * b</t>
+  </si>
+  <si>
+    <t>Лямбда-функция умножения</t>
+  </si>
+  <si>
+    <t>films = ['Titanic', 'Avatar', 'Формула Любви', 'Гардемарины', 'American Beauty', 'War and Peace', 'Stranger']
+users = {1: ['Titanic', 'Avatar'], 2: ['Формула', 'Avatar'], 3: ['Titanic', 'American Beauty'],
+         4: ['Формула Любви', 'Гардемарины'], 5: ['Avatar', 'American Beauty'], 6: ['War and Peace', 'American Beauty'], 7: ['Гардемарины', 'Формула Любви']}
+matrix = ([1 if f in users[u] else 0 for u in users] for f in films)</t>
+  </si>
+  <si>
+    <t>Сделать ГЕНЕРАТОР матрицы из 0 и 1: 1 -если юзер посмотрел фильм, 0 - если нет.</t>
+  </si>
+  <si>
+    <t>class Gen:
+    def __init__(self):
+        self.gen = ([1 if f in users[u] else 0 for u in users] for f in films)</t>
+  </si>
+  <si>
+    <t>compressed = [(i, j) for (i, row) in enumerate(list(Gen().gen)) for (j, x) in enumerate(row) if x == 1]</t>
+  </si>
+  <si>
+    <t>Создание листа туплов как координат значений, равных 1, в матрице из нулей и единиц.  Аналог sparse, но без столбца со значениями (так как они все равны 1).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Класс, создающий </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>многоразовый</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> генератор матрицы из нулей и единиц по условиям вышеописанным</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -693,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -701,9 +754,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -738,6 +788,18 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1028,43 +1090,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="45.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="41" style="8" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="45.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="41" style="7" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1072,92 +1134,92 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="5"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
+      <c r="C25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1169,216 +1231,228 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="60.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="18" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:2" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+    </row>
+    <row r="12" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="14"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="14"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1391,7 +1465,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="A1:B15"/>
+      <selection activeCell="B5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1400,72 +1474,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1476,83 +1546,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="61.28515625" style="14" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="14"/>
+    <col min="1" max="2" width="61.28515625" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
+      <c r="B2" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>